<commit_message>
Signed-off-by: Saprative Jana <saprative@gmail.com>
basic setup done
</commit_message>
<xml_diff>
--- a/trading.xlsx
+++ b/trading.xlsx
@@ -1,13 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\algo_trading\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45B52D2F-F20F-47F8-A185-6C66B8FA2F7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="3924" yWindow="1392" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Watchlist" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -18,8 +24,40 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+  <si>
+    <t>SBIN</t>
+  </si>
+  <si>
+    <t>Close</t>
+  </si>
+  <si>
+    <t>EMA(50)</t>
+  </si>
+  <si>
+    <t>EMA(200)</t>
+  </si>
+  <si>
+    <t>RSI(14)</t>
+  </si>
+  <si>
+    <t>HDFCBANK</t>
+  </si>
+  <si>
+    <t>ICICIBANK</t>
+  </si>
+  <si>
+    <t>ZOMATO</t>
+  </si>
+  <si>
+    <t>Scripts</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -29,12 +67,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -49,8 +93,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,13 +375,92 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>47.78</v>
+      </c>
+      <c r="D2">
+        <v>466.85</v>
+      </c>
+      <c r="E2">
+        <v>471.57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>39.65</v>
+      </c>
+      <c r="D3">
+        <v>1382.92</v>
+      </c>
+      <c r="E3">
+        <v>1396.07</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4">
+        <v>33.11</v>
+      </c>
+      <c r="D4">
+        <v>748.14</v>
+      </c>
+      <c r="E4">
+        <v>752.96</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5">
+        <v>62.39</v>
+      </c>
+      <c r="D5">
+        <v>76.64</v>
+      </c>
+      <c r="E5">
+        <v>73.97</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>